<commit_message>
Alteracao na planilha de dados
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -5,22 +5,35 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Mauá\Ano_2\Semestre_3\CIC_203_Algoritmos_Estrutura_de_Dados_e_Programacao\Atividades\Atividade_01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Mauá\Ano_2\Semestre_3\CIC_203_Algoritmos_Estrutura_de_Dados_e_Programacao\Atividades\Atividade_01\T1---CIC203---Algoritmos--Estrutura-de-Dados-e-Programa--o\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AB4CCE-97C6-43E7-8310-F40AF4D1DFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E386520C-7AF8-4877-81F3-D9B384BCDE19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4870" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4870" uniqueCount="18">
   <si>
     <t>DESKTOP-LSTUBER</t>
   </si>
@@ -71,6 +84,9 @@
   </si>
   <si>
     <t>Quantidade</t>
+  </si>
+  <si>
+    <t>CARLOS-PC</t>
   </si>
 </sst>
 </file>
@@ -634,7 +650,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -659,6 +675,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -795,7 +823,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dados!$R$2</c:f>
+              <c:f>Dados!$T$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -844,7 +872,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Dados!$Q$3:$Q$9</c:f>
+              <c:f>Dados!$S$3:$S$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -874,30 +902,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Dados!$R$3:$R$9</c:f>
+              <c:f>Dados!$T$3:$T$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>486.08</c:v>
+                  <c:v>486.08333333333331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1786.68</c:v>
+                  <c:v>1786.6833333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6245.07</c:v>
+                  <c:v>6245.0666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23826.71</c:v>
+                  <c:v>23683.454365079364</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91272.48</c:v>
+                  <c:v>91272.474999999991</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>425608.06</c:v>
+                  <c:v>425608.05641025648</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1295599.78</c:v>
+                  <c:v>1446545.3583333334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -914,7 +942,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dados!$S$2</c:f>
+              <c:f>Dados!$U$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -963,7 +991,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Dados!$Q$3:$Q$9</c:f>
+              <c:f>Dados!$S$3:$S$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -993,30 +1021,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Dados!$S$3:$S$9</c:f>
+              <c:f>Dados!$U$3:$U$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>303.48</c:v>
+                  <c:v>303.47499999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>642.04999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3406.72</c:v>
+                  <c:v>3406.7166666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11317.43</c:v>
+                  <c:v>11376.69692982456</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49039.42</c:v>
+                  <c:v>49039.416666666664</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>254793.27</c:v>
+                  <c:v>254793.27051282054</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1055461.04</c:v>
+                  <c:v>1206175.4583333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1033,7 +1061,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dados!$T$2</c:f>
+              <c:f>Dados!$V$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1082,7 +1110,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Dados!$Q$3:$Q$9</c:f>
+              <c:f>Dados!$S$3:$S$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1112,30 +1140,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Dados!$T$3:$T$9</c:f>
+              <c:f>Dados!$V$3:$V$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1836.59</c:v>
+                  <c:v>1836.5916666666669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7819.52</c:v>
+                  <c:v>7819.5166666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49349.41</c:v>
+                  <c:v>49349.408333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120212.27</c:v>
+                  <c:v>120212.26666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>485549.94</c:v>
+                  <c:v>485549.94166666665</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1933708.02</c:v>
+                  <c:v>1933708.0173076924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6994857.8399999999</c:v>
+                  <c:v>7699475.2583333328</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1237,7 +1265,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1943,13 +1971,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>179070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>1082040</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>163830</xdr:rowOff>
@@ -1978,6 +2006,20 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B95D382F-3E3A-4DA2-80EC-F4BE609C0BD6}" name="Table1" displayName="Table1" ref="A2:E2420" totalsRowShown="0">
+  <autoFilter ref="A2:E2420" xr:uid="{B95D382F-3E3A-4DA2-80EC-F4BE609C0BD6}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{C3C11828-C9D2-458E-B7C0-44A4D7F5EE17}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{2654CAC0-8798-4CBD-9510-399502F3D0EF}" name="tamanho"/>
+    <tableColumn id="3" xr3:uid="{C09E4209-8DF8-4CC3-8DE9-27C4C2B295A0}" name="tempo"/>
+    <tableColumn id="4" xr3:uid="{A18307D3-E616-4188-851C-2C40BC9263D6}" name="pc"/>
+    <tableColumn id="5" xr3:uid="{BE257162-F316-4118-B0EE-20C635B8F5E3}" name="tipo"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2277,39 +2319,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T2420"/>
+  <dimension ref="A1:V2420"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="N9" workbookViewId="0">
+      <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="10" width="28.77734375" customWidth="1"/>
-    <col min="12" max="14" width="28.77734375" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" customWidth="1"/>
-    <col min="18" max="20" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="9" max="11" width="28.77734375" customWidth="1"/>
+    <col min="14" max="16" width="28.77734375" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" customWidth="1"/>
+    <col min="20" max="22" width="28.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="H1" s="9" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H1" s="15"/>
+      <c r="I1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="11"/>
-      <c r="L1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="11"/>
-      <c r="Q1" s="9" t="s">
+      <c r="J1" s="10"/>
+      <c r="K1" s="11"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="10"/>
+      <c r="P1" s="11"/>
+      <c r="S1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="11"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="11"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2325,38 +2370,40 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="2" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R2" t="s">
-        <v>8</v>
-      </c>
-      <c r="S2" t="s">
-        <v>9</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>294</v>
       </c>
@@ -2373,23 +2420,30 @@
         <v>10</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="J3" s="3"/>
-      <c r="L3" s="2"/>
-      <c r="N3" s="3"/>
-      <c r="Q3" s="2">
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="3"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="3"/>
+      <c r="S3" s="2">
         <v>40000</v>
       </c>
-      <c r="R3">
-        <v>486.08</v>
-      </c>
-      <c r="S3">
-        <v>303.48</v>
-      </c>
-      <c r="T3" s="3">
-        <v>1836.59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T3" s="16">
+        <f>(I4+N4+I16+N16+I28+N28)/6</f>
+        <v>486.08333333333331</v>
+      </c>
+      <c r="U3" s="16">
+        <f t="shared" ref="U3:V3" si="0">(J4+O4+J16+O16+J28+O28)/6</f>
+        <v>303.47499999999997</v>
+      </c>
+      <c r="V3" s="17">
+        <f t="shared" si="0"/>
+        <v>1836.5916666666669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>295</v>
       </c>
@@ -2405,39 +2459,54 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="2">
         <v>40000</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="13">
+        <f>SUMIFS($C$3:$C$2420,$B$3:$B$2420,H4,$D$3:$D$2420,$I$1,$E$3:$E$2420,I$2)/COUNTIFS($B$3:$B$2420,H4,$D$3:$D$2420,$I$1,$E$3:$E$2420,I$2)</f>
+        <v>319.8</v>
+      </c>
+      <c r="J4" s="13">
+        <f>SUMIFS($C$3:$C$2420,$B$3:$B$2420,H4,$D$3:$D$2420,$I$1,$E$3:$E$2420,J$2)/COUNTIFS($B$3:$B$2420,H4,$D$3:$D$2420,$I$1,$E$3:$E$2420,J$2)</f>
+        <v>274.89999999999998</v>
+      </c>
+      <c r="K4" s="3">
+        <f>SUMIFS($C$3:$C$2420,$B$3:$B$2420,H4,$D$3:$D$2420,$I$1,$E$3:$E$2420,K$2)/COUNTIFS($B$3:$B$2420,H4,$D$3:$D$2420,$I$1,$E$3:$E$2420,K$2)</f>
+        <v>1708.6</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="2">
         <v>40000</v>
       </c>
-      <c r="J4" s="5">
-        <v>40000</v>
-      </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="4">
-        <v>40000</v>
-      </c>
-      <c r="M4" s="1">
-        <v>40000</v>
-      </c>
-      <c r="N4" s="5">
-        <v>40000</v>
-      </c>
-      <c r="Q4" s="2">
+      <c r="N4" s="13">
+        <f>SUMIFS($C$3:$C$2420,$B$3:$B$2420,$M4,$D$3:$D$2420,$N$1,$E$3:$E$2420,N$2)/COUNTIFS($B$3:$B$2420,$M4,$D$3:$D$2420,$N$1,$E$3:$E$2420,N$2)</f>
+        <v>269.5</v>
+      </c>
+      <c r="O4" s="13">
+        <f t="shared" ref="O4:P10" si="1">SUMIFS($C$3:$C$2420,$B$3:$B$2420,$M4,$D$3:$D$2420,$N$1,$E$3:$E$2420,O$2)/COUNTIFS($B$3:$B$2420,$M4,$D$3:$D$2420,$N$1,$E$3:$E$2420,O$2)</f>
+        <v>224.25</v>
+      </c>
+      <c r="P4" s="3">
+        <f t="shared" si="1"/>
+        <v>1220.55</v>
+      </c>
+      <c r="S4" s="2">
         <v>80000</v>
       </c>
-      <c r="R4">
-        <v>1786.68</v>
-      </c>
-      <c r="S4">
+      <c r="T4" s="16">
+        <f t="shared" ref="T4:T9" si="2">(I5+N5+I17+N17+I29+N29)/6</f>
+        <v>1786.6833333333334</v>
+      </c>
+      <c r="U4" s="16">
+        <f t="shared" ref="U4:U9" si="3">(J5+O5+J17+O17+J29+O29)/6</f>
         <v>642.04999999999995</v>
       </c>
-      <c r="T4" s="3">
-        <v>7819.52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V4" s="17">
+        <f t="shared" ref="V4:V9" si="4">(K5+P5+K17+P17+K29+P29)/6</f>
+        <v>7819.5166666666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>296</v>
       </c>
@@ -2454,37 +2523,52 @@
         <v>8</v>
       </c>
       <c r="H5" s="2">
-        <v>319.8</v>
-      </c>
-      <c r="I5">
-        <v>274.89999999999998</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1708.6</v>
-      </c>
-      <c r="L5" s="2">
-        <v>269.5</v>
-      </c>
-      <c r="M5">
-        <v>224.25</v>
-      </c>
-      <c r="N5" s="3">
-        <v>1220.55</v>
-      </c>
-      <c r="Q5" s="2">
+        <v>80000</v>
+      </c>
+      <c r="I5" s="13">
+        <f>SUMIFS($C$3:$C$2420,$B$3:$B$2420,H5,$D$3:$D$2420,$I$1,$E$3:$E$2420,I$2)/COUNTIFS($B$3:$B$2420,H5,$D$3:$D$2420,$I$1,$E$3:$E$2420,I$2)</f>
+        <v>1223.45</v>
+      </c>
+      <c r="J5" s="13">
+        <f t="shared" ref="J5:J10" si="5">SUMIFS($C$3:$C$2420,$B$3:$B$2420,H5,$D$3:$D$2420,$I$1,$E$3:$E$2420,J$2)/COUNTIFS($B$3:$B$2420,H5,$D$3:$D$2420,$I$1,$E$3:$E$2420,J$2)</f>
+        <v>510.3</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" ref="K5:K10" si="6">SUMIFS($C$3:$C$2420,$B$3:$B$2420,H5,$D$3:$D$2420,$I$1,$E$3:$E$2420,K$2)/COUNTIFS($B$3:$B$2420,H5,$D$3:$D$2420,$I$1,$E$3:$E$2420,K$2)</f>
+        <v>6901.45</v>
+      </c>
+      <c r="M5" s="2">
+        <v>80000</v>
+      </c>
+      <c r="N5" s="13">
+        <f t="shared" ref="N5:N10" si="7">SUMIFS($C$3:$C$2420,$B$3:$B$2420,M5,$D$3:$D$2420,$N$1,$E$3:$E$2420,N$2)/COUNTIFS($B$3:$B$2420,M5,$D$3:$D$2420,$N$1,$E$3:$E$2420,N$2)</f>
+        <v>1062.55</v>
+      </c>
+      <c r="O5" s="13">
+        <f t="shared" si="1"/>
+        <v>439.35</v>
+      </c>
+      <c r="P5" s="3">
+        <f t="shared" si="1"/>
+        <v>5481.3</v>
+      </c>
+      <c r="S5" s="2">
         <v>160000</v>
       </c>
-      <c r="R5">
-        <v>6245.07</v>
-      </c>
-      <c r="S5">
-        <v>3406.72</v>
-      </c>
-      <c r="T5" s="3">
-        <v>49349.41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T5" s="16">
+        <f t="shared" si="2"/>
+        <v>6245.0666666666666</v>
+      </c>
+      <c r="U5" s="16">
+        <f t="shared" si="3"/>
+        <v>3406.7166666666667</v>
+      </c>
+      <c r="V5" s="17">
+        <f t="shared" si="4"/>
+        <v>49349.408333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>297</v>
       </c>
@@ -2500,39 +2584,54 @@
       <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="4">
-        <v>80000</v>
-      </c>
-      <c r="I6" s="1">
-        <v>80000</v>
-      </c>
-      <c r="J6" s="5">
-        <v>80000</v>
-      </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="4">
-        <v>80000</v>
-      </c>
-      <c r="M6" s="1">
-        <v>80000</v>
-      </c>
-      <c r="N6" s="5">
-        <v>80000</v>
-      </c>
-      <c r="Q6" s="2">
+      <c r="H6" s="2">
+        <v>160000</v>
+      </c>
+      <c r="I6" s="13">
+        <f>SUMIFS($C$3:$C$2420,$B$3:$B$2420,H6,$D$3:$D$2420,$I$1,$E$3:$E$2420,I$2)/COUNTIFS($B$3:$B$2420,H6,$D$3:$D$2420,$I$1,$E$3:$E$2420,I$2)</f>
+        <v>5068.7</v>
+      </c>
+      <c r="J6" s="13">
+        <f t="shared" si="5"/>
+        <v>2276.75</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="6"/>
+        <v>28180.85</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="2">
+        <v>160000</v>
+      </c>
+      <c r="N6" s="13">
+        <f t="shared" si="7"/>
+        <v>4345.55</v>
+      </c>
+      <c r="O6" s="13">
+        <f t="shared" si="1"/>
+        <v>1807.9</v>
+      </c>
+      <c r="P6" s="3">
+        <f t="shared" si="1"/>
+        <v>23385.35</v>
+      </c>
+      <c r="S6" s="2">
         <v>320000</v>
       </c>
-      <c r="R6">
-        <v>23826.71</v>
-      </c>
-      <c r="S6">
-        <v>11317.43</v>
-      </c>
-      <c r="T6" s="3">
-        <v>120212.27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T6" s="16">
+        <f t="shared" si="2"/>
+        <v>23683.454365079364</v>
+      </c>
+      <c r="U6" s="16">
+        <f t="shared" si="3"/>
+        <v>11376.69692982456</v>
+      </c>
+      <c r="V6" s="17">
+        <f t="shared" si="4"/>
+        <v>120212.26666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>298</v>
       </c>
@@ -2549,37 +2648,52 @@
         <v>9</v>
       </c>
       <c r="H7" s="2">
-        <v>1223.45</v>
-      </c>
-      <c r="I7">
-        <v>510.3</v>
-      </c>
-      <c r="J7" s="3">
-        <v>6901.45</v>
-      </c>
-      <c r="L7" s="2">
-        <v>1062.55</v>
-      </c>
-      <c r="M7">
-        <v>439.35</v>
-      </c>
-      <c r="N7" s="3">
-        <v>5481.3</v>
-      </c>
-      <c r="Q7" s="2">
+        <v>320000</v>
+      </c>
+      <c r="I7" s="13">
+        <f t="shared" ref="I7:I10" si="8">SUMIFS($C$3:$C$2420,$B$3:$B$2420,H7,$D$3:$D$2420,$I$1,$E$3:$E$2420,I$2)/COUNTIFS($B$3:$B$2420,H7,$D$3:$D$2420,$I$1,$E$3:$E$2420,I$2)</f>
+        <v>19684.900000000001</v>
+      </c>
+      <c r="J7" s="13">
+        <f t="shared" si="5"/>
+        <v>8380.65</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="6"/>
+        <v>110801.8</v>
+      </c>
+      <c r="M7" s="2">
+        <v>320000</v>
+      </c>
+      <c r="N7" s="13">
+        <f t="shared" si="7"/>
+        <v>17190.476190476191</v>
+      </c>
+      <c r="O7" s="13">
+        <f t="shared" si="1"/>
+        <v>7111.6315789473683</v>
+      </c>
+      <c r="P7" s="3">
+        <f t="shared" si="1"/>
+        <v>93324.55</v>
+      </c>
+      <c r="S7" s="2">
         <v>640000</v>
       </c>
-      <c r="R7">
-        <v>91272.48</v>
-      </c>
-      <c r="S7">
-        <v>49039.42</v>
-      </c>
-      <c r="T7" s="3">
-        <v>485549.94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T7" s="16">
+        <f t="shared" si="2"/>
+        <v>91272.474999999991</v>
+      </c>
+      <c r="U7" s="16">
+        <f t="shared" si="3"/>
+        <v>49039.416666666664</v>
+      </c>
+      <c r="V7" s="17">
+        <f t="shared" si="4"/>
+        <v>485549.94166666665</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>299</v>
       </c>
@@ -2595,39 +2709,54 @@
       <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="4">
-        <v>160000</v>
-      </c>
-      <c r="I8" s="1">
-        <v>160000</v>
-      </c>
-      <c r="J8" s="5">
-        <v>160000</v>
-      </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="4">
-        <v>160000</v>
-      </c>
-      <c r="M8" s="1">
-        <v>160000</v>
-      </c>
-      <c r="N8" s="5">
-        <v>160000</v>
-      </c>
-      <c r="Q8" s="2">
+      <c r="H8" s="2">
+        <v>640000</v>
+      </c>
+      <c r="I8" s="13">
+        <f t="shared" si="8"/>
+        <v>78807.7</v>
+      </c>
+      <c r="J8" s="13">
+        <f t="shared" si="5"/>
+        <v>33817.050000000003</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="6"/>
+        <v>444468.5</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="2">
+        <v>640000</v>
+      </c>
+      <c r="N8" s="13">
+        <f t="shared" si="7"/>
+        <v>68434</v>
+      </c>
+      <c r="O8" s="13">
+        <f t="shared" si="1"/>
+        <v>31555.05</v>
+      </c>
+      <c r="P8" s="3">
+        <f t="shared" si="1"/>
+        <v>372328.9</v>
+      </c>
+      <c r="S8" s="2">
         <v>1280000</v>
       </c>
-      <c r="R8">
-        <v>425608.06</v>
-      </c>
-      <c r="S8">
-        <v>254793.27</v>
-      </c>
-      <c r="T8" s="3">
-        <v>1933708.02</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T8" s="16">
+        <f t="shared" si="2"/>
+        <v>425608.05641025648</v>
+      </c>
+      <c r="U8" s="16">
+        <f t="shared" si="3"/>
+        <v>254793.27051282054</v>
+      </c>
+      <c r="V8" s="17">
+        <f t="shared" si="4"/>
+        <v>1933708.0173076924</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>300</v>
       </c>
@@ -2644,37 +2773,52 @@
         <v>10</v>
       </c>
       <c r="H9" s="2">
-        <v>5068.7</v>
-      </c>
-      <c r="I9">
-        <v>2276.75</v>
-      </c>
-      <c r="J9" s="3">
-        <v>28180.85</v>
-      </c>
-      <c r="L9" s="2">
-        <v>4345.55</v>
-      </c>
-      <c r="M9">
-        <v>1807.9</v>
-      </c>
-      <c r="N9" s="3">
-        <v>23385.35</v>
-      </c>
-      <c r="Q9" s="6">
+        <v>1280000</v>
+      </c>
+      <c r="I9" s="13">
+        <f t="shared" si="8"/>
+        <v>319943.75</v>
+      </c>
+      <c r="J9" s="13">
+        <f t="shared" si="5"/>
+        <v>138033.1</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="6"/>
+        <v>1787342.9</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1280000</v>
+      </c>
+      <c r="N9" s="13">
+        <f t="shared" si="7"/>
+        <v>273472</v>
+      </c>
+      <c r="O9" s="13">
+        <f t="shared" si="1"/>
+        <v>114038.5</v>
+      </c>
+      <c r="P9" s="3">
+        <f t="shared" si="1"/>
+        <v>1488236</v>
+      </c>
+      <c r="S9" s="6">
         <v>2560000</v>
       </c>
-      <c r="R9" s="7">
-        <v>1295599.78</v>
-      </c>
-      <c r="S9" s="7">
-        <v>1055461.04</v>
-      </c>
-      <c r="T9" s="8">
-        <v>6994857.8399999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T9" s="18">
+        <f t="shared" si="2"/>
+        <v>1446545.3583333334</v>
+      </c>
+      <c r="U9" s="18">
+        <f t="shared" si="3"/>
+        <v>1206175.4583333333</v>
+      </c>
+      <c r="V9" s="19">
+        <f t="shared" si="4"/>
+        <v>7699475.2583333328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>301</v>
       </c>
@@ -2690,27 +2834,39 @@
       <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="4">
-        <v>320000</v>
-      </c>
-      <c r="I10" s="1">
-        <v>320000</v>
-      </c>
-      <c r="J10" s="5">
-        <v>320000</v>
-      </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="4">
-        <v>320000</v>
-      </c>
-      <c r="M10" s="1">
-        <v>320000</v>
-      </c>
-      <c r="N10" s="5">
-        <v>320000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H10" s="6">
+        <v>2560000</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="8"/>
+        <v>1295828.6000000001</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="5"/>
+        <v>1102191.45</v>
+      </c>
+      <c r="K10" s="8">
+        <f t="shared" si="6"/>
+        <v>7226218.2999999998</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="6">
+        <v>2560000</v>
+      </c>
+      <c r="N10" s="7">
+        <f t="shared" si="7"/>
+        <v>1098545</v>
+      </c>
+      <c r="O10" s="7">
+        <f t="shared" si="1"/>
+        <v>457760</v>
+      </c>
+      <c r="P10" s="8">
+        <f t="shared" si="1"/>
+        <v>5942384.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>302</v>
       </c>
@@ -2726,26 +2882,14 @@
       <c r="E11" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="2">
-        <v>19684.900000000001</v>
-      </c>
-      <c r="I11">
-        <v>8380.65</v>
-      </c>
-      <c r="J11" s="3">
-        <v>110801.8</v>
-      </c>
-      <c r="L11" s="2">
-        <v>18050</v>
-      </c>
-      <c r="M11">
-        <v>6756.05</v>
-      </c>
-      <c r="N11" s="3">
-        <v>93324.55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+    </row>
+    <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>303</v>
       </c>
@@ -2761,27 +2905,16 @@
       <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="4">
-        <v>640000</v>
-      </c>
-      <c r="I12" s="1">
-        <v>640000</v>
-      </c>
-      <c r="J12" s="5">
-        <v>640000</v>
-      </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="4">
-        <v>640000</v>
-      </c>
-      <c r="M12" s="1">
-        <v>640000</v>
-      </c>
-      <c r="N12" s="5">
-        <v>640000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>304</v>
       </c>
@@ -2797,26 +2930,20 @@
       <c r="E13" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="2">
-        <v>78807.7</v>
-      </c>
-      <c r="I13">
-        <v>33817.050000000003</v>
-      </c>
-      <c r="J13" s="3">
-        <v>444468.5</v>
-      </c>
-      <c r="L13" s="2">
-        <v>68434</v>
-      </c>
-      <c r="M13">
-        <v>31555.05</v>
-      </c>
-      <c r="N13" s="3">
-        <v>372328.9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H13" s="15"/>
+      <c r="I13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13" s="10"/>
+      <c r="P13" s="11"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>305</v>
       </c>
@@ -2832,27 +2959,29 @@
       <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="4">
-        <v>1280000</v>
-      </c>
-      <c r="I14" s="1">
-        <v>1280000</v>
-      </c>
-      <c r="J14" s="5">
-        <v>1280000</v>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="L14" s="4">
-        <v>1280000</v>
-      </c>
-      <c r="M14" s="1">
-        <v>1280000</v>
-      </c>
-      <c r="N14" s="5">
-        <v>1280000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H14" s="2"/>
+      <c r="I14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="O14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>306</v>
       </c>
@@ -2868,26 +2997,16 @@
       <c r="E15" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="2">
-        <v>319943.75</v>
-      </c>
-      <c r="I15">
-        <v>138033.1</v>
-      </c>
-      <c r="J15" s="3">
-        <v>1787342.9</v>
-      </c>
-      <c r="L15" s="2">
-        <v>273472</v>
-      </c>
-      <c r="M15">
-        <v>114038.5</v>
-      </c>
-      <c r="N15" s="3">
-        <v>1488236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H15" s="2"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="3"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>307</v>
       </c>
@@ -2903,27 +3022,39 @@
       <c r="E16" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="4">
-        <v>2560000</v>
-      </c>
-      <c r="I16" s="1">
-        <v>2560000</v>
-      </c>
-      <c r="J16" s="5">
-        <v>2560000</v>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="4">
-        <v>2560000</v>
-      </c>
-      <c r="M16" s="1">
-        <v>2560000</v>
-      </c>
-      <c r="N16" s="5">
-        <v>2560000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H16" s="2">
+        <v>40000</v>
+      </c>
+      <c r="I16" s="13">
+        <f>SUMIFS($C$3:$C$2420,$B$3:$B$2420,$H16,$D$3:$D$2420,$I$13,$E$3:$E$2420,I$2)/COUNTIFS($B$3:$B$2420,$H16,$D$3:$D$2420,$I$13,$E$3:$E$2420,I$2)</f>
+        <v>270.95</v>
+      </c>
+      <c r="J16" s="13">
+        <f>SUMIFS($C$3:$C$2420,$B$3:$B$2420,$H16,$D$3:$D$2420,$I$13,$E$3:$E$2420,J$2)/COUNTIFS($B$3:$B$2420,$H16,$D$3:$D$2420,$I$13,$E$3:$E$2420,J$2)</f>
+        <v>277.35000000000002</v>
+      </c>
+      <c r="K16" s="3">
+        <f>SUMIFS($C$3:$C$2420,$B$3:$B$2420,$H16,$D$3:$D$2420,$I$13,$E$3:$E$2420,K$2)/COUNTIFS($B$3:$B$2420,$H16,$D$3:$D$2420,$I$13,$E$3:$E$2420,K$2)</f>
+        <v>1616.95</v>
+      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" s="2">
+        <v>40000</v>
+      </c>
+      <c r="N16" s="13">
+        <f>SUMIFS($C$3:$C$2420,$B$3:$B$2420,$M16,$D$3:$D$2420,$N$13,$E$3:$E$2420,N$2)/COUNTIFS($B$3:$B$2420,$M16,$D$3:$D$2420,$N$13,$E$3:$E$2420,N$2)</f>
+        <v>1179.05</v>
+      </c>
+      <c r="O16" s="13">
+        <f t="shared" ref="O16:P22" si="9">SUMIFS($C$3:$C$2420,$B$3:$B$2420,$M16,$D$3:$D$2420,$N$13,$E$3:$E$2420,O$2)/COUNTIFS($B$3:$B$2420,$M16,$D$3:$D$2420,$N$13,$E$3:$E$2420,O$2)</f>
+        <v>307.8</v>
+      </c>
+      <c r="P16" s="3">
+        <f t="shared" si="9"/>
+        <v>1996.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>308</v>
       </c>
@@ -2939,26 +3070,38 @@
       <c r="E17" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="6">
-        <v>1295828.6000000001</v>
-      </c>
-      <c r="I17" s="7">
-        <v>1102191.45</v>
-      </c>
-      <c r="J17" s="8">
-        <v>7226218.2999999998</v>
-      </c>
-      <c r="L17" s="6">
-        <v>1098545</v>
-      </c>
-      <c r="M17" s="7">
-        <v>457760</v>
-      </c>
-      <c r="N17" s="8">
-        <v>5942384.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H17" s="2">
+        <v>80000</v>
+      </c>
+      <c r="I17" s="13">
+        <f t="shared" ref="I17:K22" si="10">SUMIFS($C$3:$C$2420,$B$3:$B$2420,$H17,$D$3:$D$2420,$I$13,$E$3:$E$2420,I$2)/COUNTIFS($B$3:$B$2420,$H17,$D$3:$D$2420,$I$13,$E$3:$E$2420,I$2)</f>
+        <v>1855.85</v>
+      </c>
+      <c r="J17" s="13">
+        <f t="shared" si="10"/>
+        <v>656.8</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="10"/>
+        <v>9713</v>
+      </c>
+      <c r="M17" s="2">
+        <v>80000</v>
+      </c>
+      <c r="N17" s="13">
+        <f t="shared" ref="N17:N22" si="11">SUMIFS($C$3:$C$2420,$B$3:$B$2420,$M17,$D$3:$D$2420,$N$13,$E$3:$E$2420,N$2)/COUNTIFS($B$3:$B$2420,$M17,$D$3:$D$2420,$N$13,$E$3:$E$2420,N$2)</f>
+        <v>2968.35</v>
+      </c>
+      <c r="O17" s="13">
+        <f t="shared" si="9"/>
+        <v>829.5</v>
+      </c>
+      <c r="P17" s="3">
+        <f t="shared" si="9"/>
+        <v>6878.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>309</v>
       </c>
@@ -2974,8 +3117,38 @@
       <c r="E18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H18" s="2">
+        <v>160000</v>
+      </c>
+      <c r="I18" s="13">
+        <f t="shared" si="10"/>
+        <v>4373.6499999999996</v>
+      </c>
+      <c r="J18" s="13">
+        <f t="shared" si="10"/>
+        <v>4519.1499999999996</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" si="10"/>
+        <v>27545.15</v>
+      </c>
+      <c r="M18" s="2">
+        <v>160000</v>
+      </c>
+      <c r="N18" s="13">
+        <f t="shared" si="11"/>
+        <v>9034.5</v>
+      </c>
+      <c r="O18" s="13">
+        <f t="shared" si="9"/>
+        <v>2659.65</v>
+      </c>
+      <c r="P18" s="3">
+        <f t="shared" si="9"/>
+        <v>27368.85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>310</v>
       </c>
@@ -2991,18 +3164,38 @@
       <c r="E19" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="11"/>
-      <c r="L19" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="M19" s="10"/>
-      <c r="N19" s="11"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H19" s="2">
+        <v>320000</v>
+      </c>
+      <c r="I19" s="13">
+        <f t="shared" si="10"/>
+        <v>18367.25</v>
+      </c>
+      <c r="J19" s="13">
+        <f t="shared" si="10"/>
+        <v>6910.55</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" si="10"/>
+        <v>115261.9</v>
+      </c>
+      <c r="M19" s="2">
+        <v>320000</v>
+      </c>
+      <c r="N19" s="13">
+        <f t="shared" si="11"/>
+        <v>32565.35</v>
+      </c>
+      <c r="O19" s="13">
+        <f t="shared" si="9"/>
+        <v>10025.75</v>
+      </c>
+      <c r="P19" s="3">
+        <f t="shared" si="9"/>
+        <v>110937.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>311</v>
       </c>
@@ -3018,26 +3211,38 @@
       <c r="E20" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M20" t="s">
-        <v>9</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H20" s="2">
+        <v>640000</v>
+      </c>
+      <c r="I20" s="13">
+        <f t="shared" si="10"/>
+        <v>69265.649999999994</v>
+      </c>
+      <c r="J20" s="13">
+        <f t="shared" si="10"/>
+        <v>25894.45</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="10"/>
+        <v>438166</v>
+      </c>
+      <c r="M20" s="2">
+        <v>640000</v>
+      </c>
+      <c r="N20" s="13">
+        <f t="shared" si="11"/>
+        <v>109899.8</v>
+      </c>
+      <c r="O20" s="13">
+        <f t="shared" si="9"/>
+        <v>75535.649999999994</v>
+      </c>
+      <c r="P20" s="3">
+        <f t="shared" si="9"/>
+        <v>447370.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>312</v>
       </c>
@@ -3053,12 +3258,38 @@
       <c r="E21" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="J21" s="3"/>
-      <c r="L21" s="2"/>
-      <c r="N21" s="3"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H21" s="2">
+        <v>1280000</v>
+      </c>
+      <c r="I21" s="13">
+        <f t="shared" si="10"/>
+        <v>276719.05</v>
+      </c>
+      <c r="J21" s="13">
+        <f t="shared" si="10"/>
+        <v>104145.1</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" si="10"/>
+        <v>1749314.55</v>
+      </c>
+      <c r="M21" s="2">
+        <v>1280000</v>
+      </c>
+      <c r="N21" s="13">
+        <f t="shared" si="11"/>
+        <v>339887.5</v>
+      </c>
+      <c r="O21" s="13">
+        <f t="shared" si="9"/>
+        <v>116403.5</v>
+      </c>
+      <c r="P21" s="3">
+        <f t="shared" si="9"/>
+        <v>1727885</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>313</v>
       </c>
@@ -3074,27 +3305,39 @@
       <c r="E22" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="4">
-        <v>40000</v>
-      </c>
-      <c r="I22" s="1">
-        <v>40000</v>
-      </c>
-      <c r="J22" s="5">
-        <v>40000</v>
-      </c>
-      <c r="K22" s="1"/>
-      <c r="L22" s="4">
-        <v>40000</v>
-      </c>
-      <c r="M22" s="1">
-        <v>40000</v>
-      </c>
-      <c r="N22" s="5">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H22" s="6">
+        <v>2560000</v>
+      </c>
+      <c r="I22" s="7">
+        <f t="shared" si="10"/>
+        <v>1204020.05</v>
+      </c>
+      <c r="J22" s="7">
+        <f t="shared" si="10"/>
+        <v>1280787.3</v>
+      </c>
+      <c r="K22" s="8">
+        <f t="shared" si="10"/>
+        <v>7118871.25</v>
+      </c>
+      <c r="L22" s="1"/>
+      <c r="M22" s="6">
+        <v>2560000</v>
+      </c>
+      <c r="N22" s="7">
+        <f t="shared" si="11"/>
+        <v>1403313.5</v>
+      </c>
+      <c r="O22" s="7">
+        <f t="shared" si="9"/>
+        <v>477706.5</v>
+      </c>
+      <c r="P22" s="8">
+        <f t="shared" si="9"/>
+        <v>6940994</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>314</v>
       </c>
@@ -3110,26 +3353,14 @@
       <c r="E23" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="2">
-        <v>270.95</v>
-      </c>
-      <c r="I23">
-        <v>277.35000000000002</v>
-      </c>
-      <c r="J23" s="3">
-        <v>1616.95</v>
-      </c>
-      <c r="L23" s="2">
-        <v>1179.05</v>
-      </c>
-      <c r="M23">
-        <v>307.8</v>
-      </c>
-      <c r="N23" s="3">
-        <v>1996.4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+    </row>
+    <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>315</v>
       </c>
@@ -3145,27 +3376,16 @@
       <c r="E24" t="s">
         <v>10</v>
       </c>
-      <c r="H24" s="4">
-        <v>80000</v>
-      </c>
-      <c r="I24" s="1">
-        <v>80000</v>
-      </c>
-      <c r="J24" s="5">
-        <v>80000</v>
-      </c>
-      <c r="K24" s="1"/>
-      <c r="L24" s="4">
-        <v>80000</v>
-      </c>
-      <c r="M24" s="1">
-        <v>80000</v>
-      </c>
-      <c r="N24" s="5">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>316</v>
       </c>
@@ -3181,26 +3401,20 @@
       <c r="E25" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="2">
-        <v>1855.85</v>
-      </c>
-      <c r="I25">
-        <v>656.8</v>
-      </c>
-      <c r="J25" s="3">
-        <v>9713</v>
-      </c>
-      <c r="L25" s="2">
-        <v>2968.35</v>
-      </c>
-      <c r="M25">
-        <v>829.5</v>
-      </c>
-      <c r="N25" s="3">
-        <v>6878.25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H25" s="15"/>
+      <c r="I25" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="10"/>
+      <c r="K25" s="11"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" s="10"/>
+      <c r="P25" s="11"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>317</v>
       </c>
@@ -3216,27 +3430,29 @@
       <c r="E26" t="s">
         <v>8</v>
       </c>
-      <c r="H26" s="4">
-        <v>160000</v>
-      </c>
-      <c r="I26" s="1">
-        <v>160000</v>
-      </c>
-      <c r="J26" s="5">
-        <v>160000</v>
-      </c>
-      <c r="K26" s="1"/>
-      <c r="L26" s="4">
-        <v>160000</v>
-      </c>
-      <c r="M26" s="1">
-        <v>160000</v>
-      </c>
-      <c r="N26" s="5">
-        <v>160000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H26" s="2"/>
+      <c r="I26" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="O26" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>318</v>
       </c>
@@ -3252,26 +3468,16 @@
       <c r="E27" t="s">
         <v>10</v>
       </c>
-      <c r="H27" s="2">
-        <v>4373.6499999999996</v>
-      </c>
-      <c r="I27">
-        <v>4519.1499999999996</v>
-      </c>
-      <c r="J27" s="3">
-        <v>27545.15</v>
-      </c>
-      <c r="L27" s="2">
-        <v>9034.5</v>
-      </c>
-      <c r="M27">
-        <v>2659.65</v>
-      </c>
-      <c r="N27" s="3">
-        <v>27368.85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H27" s="2"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="3"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>319</v>
       </c>
@@ -3287,27 +3493,39 @@
       <c r="E28" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="4">
-        <v>320000</v>
-      </c>
-      <c r="I28" s="1">
-        <v>320000</v>
-      </c>
-      <c r="J28" s="5">
-        <v>320000</v>
-      </c>
-      <c r="K28" s="1"/>
-      <c r="L28" s="4">
-        <v>320000</v>
-      </c>
-      <c r="M28" s="1">
-        <v>320000</v>
-      </c>
-      <c r="N28" s="5">
-        <v>320000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H28" s="2">
+        <v>40000</v>
+      </c>
+      <c r="I28" s="13">
+        <f>SUMIFS($C$3:$C$2420,$B$3:$B$2420,$H28,$D$3:$D$2420,$I$25,$E$3:$E$2420,I$2)/COUNTIFS($B$3:$B$2420,$H28,$D$3:$D$2420,$I$25,$E$3:$E$2420,I$2)</f>
+        <v>496.9</v>
+      </c>
+      <c r="J28" s="13">
+        <f>SUMIFS($C$3:$C$2420,$B$3:$B$2420,$H28,$D$3:$D$2420,$I$25,$E$3:$E$2420,J$2)/COUNTIFS($B$3:$B$2420,$H28,$D$3:$D$2420,$I$25,$E$3:$E$2420,J$2)</f>
+        <v>434.15</v>
+      </c>
+      <c r="K28" s="3">
+        <f>SUMIFS($C$3:$C$2420,$B$3:$B$2420,$H28,$D$3:$D$2420,$I$25,$E$3:$E$2420,K$2)/COUNTIFS($B$3:$B$2420,$H28,$D$3:$D$2420,$I$25,$E$3:$E$2420,K$2)</f>
+        <v>2553.85</v>
+      </c>
+      <c r="L28" s="1"/>
+      <c r="M28" s="2">
+        <v>40000</v>
+      </c>
+      <c r="N28" s="13">
+        <f>SUMIFS($C$3:$C$2420,$B$3:$B$2420,$M28,$D$3:$D$2420,$N$25,$E$3:$E$2420,N$2)/COUNTIFS($B$3:$B$2420,$M28,$D$3:$D$2420,$N$25,$E$3:$E$2420,N$2)</f>
+        <v>380.3</v>
+      </c>
+      <c r="O28" s="13">
+        <f t="shared" ref="O28:P34" si="12">SUMIFS($C$3:$C$2420,$B$3:$B$2420,$M28,$D$3:$D$2420,$N$25,$E$3:$E$2420,O$2)/COUNTIFS($B$3:$B$2420,$M28,$D$3:$D$2420,$N$25,$E$3:$E$2420,O$2)</f>
+        <v>302.39999999999998</v>
+      </c>
+      <c r="P28" s="3">
+        <f t="shared" si="12"/>
+        <v>1923.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>320</v>
       </c>
@@ -3324,25 +3542,37 @@
         <v>8</v>
       </c>
       <c r="H29" s="2">
-        <v>18367.25</v>
-      </c>
-      <c r="I29">
-        <v>6910.55</v>
-      </c>
-      <c r="J29" s="3">
-        <v>115261.9</v>
-      </c>
-      <c r="L29" s="2">
-        <v>32565.35</v>
-      </c>
-      <c r="M29">
-        <v>10025.75</v>
-      </c>
-      <c r="N29" s="3">
-        <v>110937.1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+        <v>80000</v>
+      </c>
+      <c r="I29" s="13">
+        <f t="shared" ref="I29:K34" si="13">SUMIFS($C$3:$C$2420,$B$3:$B$2420,$H29,$D$3:$D$2420,$I$25,$E$3:$E$2420,I$2)/COUNTIFS($B$3:$B$2420,$H29,$D$3:$D$2420,$I$25,$E$3:$E$2420,I$2)</f>
+        <v>1939.05</v>
+      </c>
+      <c r="J29" s="13">
+        <f t="shared" si="13"/>
+        <v>806.25</v>
+      </c>
+      <c r="K29" s="3">
+        <f t="shared" si="13"/>
+        <v>9784.15</v>
+      </c>
+      <c r="M29" s="2">
+        <v>80000</v>
+      </c>
+      <c r="N29" s="13">
+        <f t="shared" ref="N29:N34" si="14">SUMIFS($C$3:$C$2420,$B$3:$B$2420,$M29,$D$3:$D$2420,$N$25,$E$3:$E$2420,N$2)/COUNTIFS($B$3:$B$2420,$M29,$D$3:$D$2420,$N$25,$E$3:$E$2420,N$2)</f>
+        <v>1670.85</v>
+      </c>
+      <c r="O29" s="13">
+        <f t="shared" si="12"/>
+        <v>610.1</v>
+      </c>
+      <c r="P29" s="3">
+        <f t="shared" si="12"/>
+        <v>8158.95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>321</v>
       </c>
@@ -3358,27 +3588,39 @@
       <c r="E30" t="s">
         <v>10</v>
       </c>
-      <c r="H30" s="4">
-        <v>640000</v>
-      </c>
-      <c r="I30" s="1">
-        <v>640000</v>
-      </c>
-      <c r="J30" s="5">
-        <v>640000</v>
-      </c>
-      <c r="K30" s="1"/>
-      <c r="L30" s="4">
-        <v>640000</v>
-      </c>
-      <c r="M30" s="1">
-        <v>640000</v>
-      </c>
-      <c r="N30" s="5">
-        <v>640000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H30" s="2">
+        <v>160000</v>
+      </c>
+      <c r="I30" s="13">
+        <f t="shared" si="13"/>
+        <v>6901.05</v>
+      </c>
+      <c r="J30" s="13">
+        <f t="shared" si="13"/>
+        <v>6296.4</v>
+      </c>
+      <c r="K30" s="3">
+        <f t="shared" si="13"/>
+        <v>39163.85</v>
+      </c>
+      <c r="L30" s="1"/>
+      <c r="M30" s="2">
+        <v>160000</v>
+      </c>
+      <c r="N30" s="13">
+        <f t="shared" si="14"/>
+        <v>7746.95</v>
+      </c>
+      <c r="O30" s="13">
+        <f t="shared" si="12"/>
+        <v>2880.45</v>
+      </c>
+      <c r="P30" s="3">
+        <f t="shared" si="12"/>
+        <v>150452.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>322</v>
       </c>
@@ -3395,25 +3637,37 @@
         <v>9</v>
       </c>
       <c r="H31" s="2">
-        <v>69265.649999999994</v>
-      </c>
-      <c r="I31">
-        <v>25894.45</v>
-      </c>
-      <c r="J31" s="3">
-        <v>438166</v>
-      </c>
-      <c r="L31" s="2">
-        <v>109899.8</v>
-      </c>
-      <c r="M31">
-        <v>75535.649999999994</v>
-      </c>
-      <c r="N31" s="3">
-        <v>447370.3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+        <v>320000</v>
+      </c>
+      <c r="I31" s="13">
+        <f t="shared" si="13"/>
+        <v>28873.5</v>
+      </c>
+      <c r="J31" s="13">
+        <f t="shared" si="13"/>
+        <v>26523.85</v>
+      </c>
+      <c r="K31" s="3">
+        <f t="shared" si="13"/>
+        <v>161769.65</v>
+      </c>
+      <c r="M31" s="2">
+        <v>320000</v>
+      </c>
+      <c r="N31" s="13">
+        <f t="shared" si="14"/>
+        <v>25419.25</v>
+      </c>
+      <c r="O31" s="13">
+        <f t="shared" si="12"/>
+        <v>9307.75</v>
+      </c>
+      <c r="P31" s="3">
+        <f t="shared" si="12"/>
+        <v>129178.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>323</v>
       </c>
@@ -3429,27 +3683,39 @@
       <c r="E32" t="s">
         <v>8</v>
       </c>
-      <c r="H32" s="4">
-        <v>1280000</v>
-      </c>
-      <c r="I32" s="1">
-        <v>1280000</v>
-      </c>
-      <c r="J32" s="5">
-        <v>1280000</v>
-      </c>
-      <c r="K32" s="1"/>
-      <c r="L32" s="4">
-        <v>1280000</v>
-      </c>
-      <c r="M32" s="1">
-        <v>1280000</v>
-      </c>
-      <c r="N32" s="5">
-        <v>1280000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H32" s="2">
+        <v>640000</v>
+      </c>
+      <c r="I32" s="13">
+        <f t="shared" si="13"/>
+        <v>116330.1</v>
+      </c>
+      <c r="J32" s="13">
+        <f t="shared" si="13"/>
+        <v>54393.7</v>
+      </c>
+      <c r="K32" s="3">
+        <f t="shared" si="13"/>
+        <v>691868.9</v>
+      </c>
+      <c r="L32" s="1"/>
+      <c r="M32" s="2">
+        <v>640000</v>
+      </c>
+      <c r="N32" s="13">
+        <f t="shared" si="14"/>
+        <v>104897.60000000001</v>
+      </c>
+      <c r="O32" s="13">
+        <f t="shared" si="12"/>
+        <v>73040.600000000006</v>
+      </c>
+      <c r="P32" s="3">
+        <f t="shared" si="12"/>
+        <v>519097.05</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>324</v>
       </c>
@@ -3466,25 +3732,37 @@
         <v>10</v>
       </c>
       <c r="H33" s="2">
-        <v>276719.05</v>
-      </c>
-      <c r="I33">
-        <v>104145.1</v>
-      </c>
-      <c r="J33" s="3">
-        <v>1749314.55</v>
-      </c>
-      <c r="L33" s="2">
-        <v>339887.5</v>
-      </c>
-      <c r="M33">
-        <v>116403.5</v>
-      </c>
-      <c r="N33" s="3">
-        <v>1727885</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1280000</v>
+      </c>
+      <c r="I33" s="13">
+        <f t="shared" si="13"/>
+        <v>909991.5384615385</v>
+      </c>
+      <c r="J33" s="13">
+        <f t="shared" si="13"/>
+        <v>597199.92307692312</v>
+      </c>
+      <c r="K33" s="3">
+        <f t="shared" si="13"/>
+        <v>2755580.153846154</v>
+      </c>
+      <c r="M33" s="2">
+        <v>1280000</v>
+      </c>
+      <c r="N33" s="13">
+        <f t="shared" si="14"/>
+        <v>433634.5</v>
+      </c>
+      <c r="O33" s="13">
+        <f t="shared" si="12"/>
+        <v>458939.5</v>
+      </c>
+      <c r="P33" s="3">
+        <f t="shared" si="12"/>
+        <v>2093889.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>325</v>
       </c>
@@ -3500,27 +3778,39 @@
       <c r="E34" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34" s="6">
         <v>2560000</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I34" s="7">
+        <f t="shared" si="13"/>
+        <v>1866218</v>
+      </c>
+      <c r="J34" s="7">
+        <f t="shared" si="13"/>
+        <v>2110034.5</v>
+      </c>
+      <c r="K34" s="8">
+        <f t="shared" si="13"/>
+        <v>10512974.5</v>
+      </c>
+      <c r="L34" s="1"/>
+      <c r="M34" s="6">
         <v>2560000</v>
       </c>
-      <c r="J34" s="5">
-        <v>2560000</v>
-      </c>
-      <c r="K34" s="1"/>
-      <c r="L34" s="4">
-        <v>2560000</v>
-      </c>
-      <c r="M34" s="1">
-        <v>2560000</v>
-      </c>
-      <c r="N34" s="5">
-        <v>2560000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N34" s="7">
+        <f t="shared" si="14"/>
+        <v>1811347</v>
+      </c>
+      <c r="O34" s="7">
+        <f t="shared" si="12"/>
+        <v>1808573</v>
+      </c>
+      <c r="P34" s="8">
+        <f t="shared" si="12"/>
+        <v>8455409</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>326</v>
       </c>
@@ -3536,26 +3826,11 @@
       <c r="E35" t="s">
         <v>8</v>
       </c>
-      <c r="H35" s="6">
-        <v>1204020.05</v>
-      </c>
-      <c r="I35" s="7">
-        <v>1280787.3</v>
-      </c>
-      <c r="J35" s="8">
-        <v>7118871.25</v>
-      </c>
-      <c r="L35" s="6">
-        <v>1403313.5</v>
-      </c>
-      <c r="M35" s="7">
-        <v>477706.5</v>
-      </c>
-      <c r="N35" s="8">
-        <v>6940994</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+    </row>
+    <row r="36" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>327</v>
       </c>
@@ -3572,7 +3847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>328</v>
       </c>
@@ -3588,18 +3863,14 @@
       <c r="E37" t="s">
         <v>9</v>
       </c>
-      <c r="H37" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" s="10"/>
-      <c r="J37" s="11"/>
-      <c r="L37" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="M37" s="10"/>
-      <c r="N37" s="11"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="11"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>329</v>
       </c>
@@ -3615,26 +3886,13 @@
       <c r="E38" t="s">
         <v>8</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I38" t="s">
-        <v>9</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M38" t="s">
-        <v>9</v>
-      </c>
-      <c r="N38" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="N38" s="2"/>
+      <c r="P38" s="3"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>330</v>
       </c>
@@ -3650,12 +3908,13 @@
       <c r="E39" t="s">
         <v>10</v>
       </c>
-      <c r="H39" s="2"/>
-      <c r="J39" s="3"/>
-      <c r="L39" s="2"/>
-      <c r="N39" s="3"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="N39" s="2"/>
+      <c r="P39" s="3"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>331</v>
       </c>
@@ -3671,27 +3930,16 @@
       <c r="E40" t="s">
         <v>9</v>
       </c>
-      <c r="H40" s="4">
-        <v>40000</v>
-      </c>
-      <c r="I40" s="1">
-        <v>40000</v>
-      </c>
-      <c r="J40" s="5">
-        <v>40000</v>
-      </c>
-      <c r="K40" s="1"/>
-      <c r="L40" s="4">
-        <v>40000</v>
-      </c>
-      <c r="M40" s="1">
-        <v>40000</v>
-      </c>
-      <c r="N40" s="5">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="5"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>332</v>
       </c>
@@ -3707,26 +3955,13 @@
       <c r="E41" t="s">
         <v>8</v>
       </c>
-      <c r="H41" s="2">
-        <v>496.9</v>
-      </c>
-      <c r="I41">
-        <v>434.15</v>
-      </c>
-      <c r="J41" s="3">
-        <v>2553.85</v>
-      </c>
-      <c r="L41" s="2">
-        <v>380.3</v>
-      </c>
-      <c r="M41">
-        <v>302.39999999999998</v>
-      </c>
-      <c r="N41" s="3">
-        <v>1923.2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="N41" s="2"/>
+      <c r="P41" s="3"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>333</v>
       </c>
@@ -3742,27 +3977,16 @@
       <c r="E42" t="s">
         <v>10</v>
       </c>
-      <c r="H42" s="4">
-        <v>80000</v>
-      </c>
-      <c r="I42" s="1">
-        <v>80000</v>
-      </c>
-      <c r="J42" s="5">
-        <v>80000</v>
-      </c>
-      <c r="K42" s="1"/>
-      <c r="L42" s="4">
-        <v>80000</v>
-      </c>
-      <c r="M42" s="1">
-        <v>80000</v>
-      </c>
-      <c r="N42" s="5">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="5"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>334</v>
       </c>
@@ -3778,26 +4002,13 @@
       <c r="E43" t="s">
         <v>9</v>
       </c>
-      <c r="H43" s="2">
-        <v>1939.05</v>
-      </c>
-      <c r="I43">
-        <v>806.25</v>
-      </c>
-      <c r="J43" s="3">
-        <v>9784.15</v>
-      </c>
-      <c r="L43" s="2">
-        <v>1670.85</v>
-      </c>
-      <c r="M43">
-        <v>610.1</v>
-      </c>
-      <c r="N43" s="3">
-        <v>8158.95</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="N43" s="2"/>
+      <c r="P43" s="3"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>335</v>
       </c>
@@ -3813,27 +4024,16 @@
       <c r="E44" t="s">
         <v>8</v>
       </c>
-      <c r="H44" s="4">
-        <v>160000</v>
-      </c>
-      <c r="I44" s="1">
-        <v>160000</v>
-      </c>
-      <c r="J44" s="5">
-        <v>160000</v>
-      </c>
-      <c r="K44" s="1"/>
-      <c r="L44" s="4">
-        <v>160000</v>
-      </c>
-      <c r="M44" s="1">
-        <v>160000</v>
-      </c>
-      <c r="N44" s="5">
-        <v>160000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="5"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>336</v>
       </c>
@@ -3849,26 +4049,13 @@
       <c r="E45" t="s">
         <v>10</v>
       </c>
-      <c r="H45" s="2">
-        <v>6901.05</v>
-      </c>
-      <c r="I45">
-        <v>6296.4</v>
-      </c>
-      <c r="J45" s="3">
-        <v>39163.85</v>
-      </c>
-      <c r="L45" s="2">
-        <v>7746.95</v>
-      </c>
-      <c r="M45">
-        <v>2880.45</v>
-      </c>
-      <c r="N45" s="3">
-        <v>150452.4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="N45" s="2"/>
+      <c r="P45" s="3"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>337</v>
       </c>
@@ -3884,27 +4071,16 @@
       <c r="E46" t="s">
         <v>9</v>
       </c>
-      <c r="H46" s="4">
-        <v>320000</v>
-      </c>
-      <c r="I46" s="1">
-        <v>320000</v>
-      </c>
-      <c r="J46" s="5">
-        <v>320000</v>
-      </c>
-      <c r="K46" s="1"/>
-      <c r="L46" s="4">
-        <v>320000</v>
-      </c>
-      <c r="M46" s="1">
-        <v>320000</v>
-      </c>
-      <c r="N46" s="5">
-        <v>320000</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="5"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>338</v>
       </c>
@@ -3920,26 +4096,13 @@
       <c r="E47" t="s">
         <v>8</v>
       </c>
-      <c r="H47" s="2">
-        <v>28873.5</v>
-      </c>
-      <c r="I47">
-        <v>26523.85</v>
-      </c>
-      <c r="J47" s="3">
-        <v>161769.65</v>
-      </c>
-      <c r="L47" s="2">
-        <v>25419.25</v>
-      </c>
-      <c r="M47">
-        <v>9307.75</v>
-      </c>
-      <c r="N47" s="3">
-        <v>129178.6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="N47" s="2"/>
+      <c r="P47" s="3"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>339</v>
       </c>
@@ -3955,27 +4118,16 @@
       <c r="E48" t="s">
         <v>10</v>
       </c>
-      <c r="H48" s="4">
-        <v>640000</v>
-      </c>
-      <c r="I48" s="1">
-        <v>640000</v>
-      </c>
-      <c r="J48" s="5">
-        <v>640000</v>
-      </c>
-      <c r="K48" s="1"/>
-      <c r="L48" s="4">
-        <v>640000</v>
-      </c>
-      <c r="M48" s="1">
-        <v>640000</v>
-      </c>
-      <c r="N48" s="5">
-        <v>640000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="5"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>340</v>
       </c>
@@ -3991,26 +4143,13 @@
       <c r="E49" t="s">
         <v>9</v>
       </c>
-      <c r="H49" s="2">
-        <v>116330.1</v>
-      </c>
-      <c r="I49">
-        <v>54393.7</v>
-      </c>
-      <c r="J49" s="3">
-        <v>691868.9</v>
-      </c>
-      <c r="L49" s="2">
-        <v>104897.60000000001</v>
-      </c>
-      <c r="M49">
-        <v>73040.600000000006</v>
-      </c>
-      <c r="N49" s="3">
-        <v>519097.05</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="N49" s="2"/>
+      <c r="P49" s="3"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>341</v>
       </c>
@@ -4026,27 +4165,16 @@
       <c r="E50" t="s">
         <v>8</v>
       </c>
-      <c r="H50" s="4">
-        <v>1280000</v>
-      </c>
-      <c r="I50" s="1">
-        <v>1280000</v>
-      </c>
-      <c r="J50" s="5">
-        <v>1280000</v>
-      </c>
-      <c r="K50" s="1"/>
-      <c r="L50" s="4">
-        <v>1280000</v>
-      </c>
-      <c r="M50" s="1">
-        <v>1280000</v>
-      </c>
-      <c r="N50" s="5">
-        <v>1280000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="5"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>342</v>
       </c>
@@ -4062,26 +4190,13 @@
       <c r="E51" t="s">
         <v>10</v>
       </c>
-      <c r="H51" s="2">
-        <v>909991.54</v>
-      </c>
-      <c r="I51">
-        <v>597199.92000000004</v>
-      </c>
-      <c r="J51" s="3">
-        <v>2755580.15</v>
-      </c>
-      <c r="L51" s="2">
-        <v>433634.5</v>
-      </c>
-      <c r="M51">
-        <v>458939.5</v>
-      </c>
-      <c r="N51" s="3">
-        <v>2093889.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="N51" s="2"/>
+      <c r="P51" s="3"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>343</v>
       </c>
@@ -4097,27 +4212,16 @@
       <c r="E52" t="s">
         <v>9</v>
       </c>
-      <c r="H52" s="4">
-        <v>2560000</v>
-      </c>
-      <c r="I52" s="1">
-        <v>2560000</v>
-      </c>
-      <c r="J52" s="5">
-        <v>2560000</v>
-      </c>
-      <c r="K52" s="1"/>
-      <c r="L52" s="4">
-        <v>2560000</v>
-      </c>
-      <c r="M52" s="1">
-        <v>2560000</v>
-      </c>
-      <c r="N52" s="5">
-        <v>2560000</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="5"/>
+    </row>
+    <row r="53" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>344</v>
       </c>
@@ -4133,26 +4237,14 @@
       <c r="E53" t="s">
         <v>8</v>
       </c>
-      <c r="H53" s="6">
-        <v>1866218</v>
-      </c>
-      <c r="I53" s="7">
-        <v>2110034.5</v>
-      </c>
-      <c r="J53" s="8">
-        <v>10512974.5</v>
-      </c>
-      <c r="L53" s="6">
-        <v>905673.5</v>
-      </c>
-      <c r="M53" s="7">
-        <v>904286.5</v>
-      </c>
-      <c r="N53" s="8">
-        <v>4227704.5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+      <c r="N53" s="6"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="8"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>345</v>
       </c>
@@ -4169,7 +4261,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>346</v>
       </c>
@@ -4186,7 +4278,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>347</v>
       </c>
@@ -4203,7 +4295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>348</v>
       </c>
@@ -4220,7 +4312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>349</v>
       </c>
@@ -4237,7 +4329,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>350</v>
       </c>
@@ -4254,7 +4346,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>351</v>
       </c>
@@ -4271,7 +4363,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>352</v>
       </c>
@@ -4288,7 +4380,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>353</v>
       </c>
@@ -4305,7 +4397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>354</v>
       </c>
@@ -4322,7 +4414,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>355</v>
       </c>
@@ -44392,16 +44484,21 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="L37:N37"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="Q1:T1"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="H19:J19"/>
+  <mergeCells count="9">
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="N37:P37"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N25:P25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>